<commit_message>
modify and reformat code
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/paymentData.xlsx
+++ b/src/test/resources/excelData/paymentData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\20212025-IT\20242025-1\IntelliJ\DemoTestNG\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F56EAED-1994-405E-B325-95775A5E02E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97212249-69CD-49CC-B01D-25A43D680D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A2D50A5-5113-41C7-A06C-6CCCB8A88FC9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2A2D50A5-5113-41C7-A06C-6CCCB8A88FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="paymentOptions" sheetId="1" r:id="rId1"/>
+    <sheet name="bookNames" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>isHaveAddress</t>
   </si>
@@ -54,16 +55,40 @@
   </si>
   <si>
     <t>customer1</t>
+  </si>
+  <si>
+    <t>bookName</t>
+  </si>
+  <si>
+    <t>CÁCH NỀN KINH TẾ VẬN HÀNH Niềm tin, sự sụp đổ và những lời tiên tri tự đúng</t>
+  </si>
+  <si>
+    <t>Lời Thú Tội Của Một Sát Thủ Kinh Tế - Bìa Cứng (Tái Bản 2023)</t>
+  </si>
+  <si>
+    <t>Tuyển tập Vũ Trọng Phụng</t>
+  </si>
+  <si>
+    <t>Tuyển Tập Truyện Ngắn Hay Nhất Của Nguyễn Minh Châu</t>
+  </si>
+  <si>
+    <t>Văn Học Trong Nhà Trường: Thơ Nguyễn Khuyến</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,8 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B1527F-8FEA-47D4-8610-572BDFA5E816}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,4 +632,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{992685C5-9153-4202-BD3C-748FA7858915}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="64" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>